<commit_message>
Adding duplicates removal script
</commit_message>
<xml_diff>
--- a/TsakonianDB/tables/sources.xlsx
+++ b/TsakonianDB/tables/sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgcha\Desktop\Python\Códigos\Tsakonian tools\TsakonianDB\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACFD845-164E-4C13-9E38-7F7922A1E06B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21EDCB0-53AE-4571-A35A-DA56AFF9697D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>source_id</t>
   </si>
@@ -37,6 +37,15 @@
   </si>
   <si>
     <t>Καμβύσης, Ιωάννης (2020). Για να κ̇οντούμε τα γρούσσα νάμου</t>
+  </si>
+  <si>
+    <t>Δέφνερ, Μιχαήλ (1923). Λεξικόν της Τσακώνικης Διαλέκτου</t>
+  </si>
+  <si>
+    <t>Warr, John. Tsakoniandialect.info</t>
+  </si>
+  <si>
+    <t>http://www.tsakoniandialect.info/</t>
   </si>
 </sst>
 </file>
@@ -92,8 +101,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2CEA5998-AB36-4F3F-B6A8-CBC43F694949}" name="Tabla1" displayName="Tabla1" ref="A1:C2" totalsRowShown="0">
-  <autoFilter ref="A1:C2" xr:uid="{2CEA5998-AB36-4F3F-B6A8-CBC43F694949}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2CEA5998-AB36-4F3F-B6A8-CBC43F694949}" name="Tabla1" displayName="Tabla1" ref="A1:C4" totalsRowShown="0">
+  <autoFilter ref="A1:C4" xr:uid="{2CEA5998-AB36-4F3F-B6A8-CBC43F694949}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{9BFE6A19-9B22-404B-A2B4-47A087E2CDFE}" name="source_id"/>
     <tableColumn id="2" xr3:uid="{81F399DD-C578-40DC-94F8-01D977ED0433}" name="title"/>
@@ -366,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,6 +406,25 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>